<commit_message>
updated the metadfata doc
</commit_message>
<xml_diff>
--- a/earthquake/static/data/earthquake-metadata.xlsx
+++ b/earthquake/static/data/earthquake-metadata.xlsx
@@ -5,24 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\project\p2-earthquake-visualization\earthquake\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\project\p2-earthquake-visualization\earthquake\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3260C4D5-9170-434A-AE81-AC7CF18B9760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A2CE61-DED6-4FFE-87BE-3E161ADBD29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11325" yWindow="2880" windowWidth="15120" windowHeight="12735" xr2:uid="{35645E97-20EB-4A3D-AEE1-C1100923BF2B}"/>
+    <workbookView xWindow="11850" yWindow="3765" windowWidth="15750" windowHeight="11085" firstSheet="1" activeTab="4" xr2:uid="{35645E97-20EB-4A3D-AEE1-C1100923BF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Region Code" sheetId="3" r:id="rId2"/>
     <sheet name="MMI Internsity" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Table columns" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Metadata!$A$1:$D$46</definedName>
     <definedName name="EQ_MAG_MS" localSheetId="3">Sheet4!$B$2</definedName>
-    <definedName name="HOUR" localSheetId="0">Metadata!$B$6</definedName>
+    <definedName name="HOUR" localSheetId="0">Metadata!$C$6</definedName>
     <definedName name="REGION_NAME" localSheetId="1">'Region Code'!$A$2</definedName>
-    <definedName name="YEAR" localSheetId="0">Metadata!$B$4</definedName>
+    <definedName name="YEAR" localSheetId="0">Metadata!$C$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="137">
   <si>
     <t>FLAG_TSUNAMI</t>
   </si>
@@ -402,6 +404,81 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>Magnitude</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>intensity</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>Date type</t>
+  </si>
+  <si>
+    <t>For Definition</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>region_cd</t>
+  </si>
+  <si>
+    <t>tsunami_fl</t>
+  </si>
+  <si>
+    <t>magnitude</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>total_deaths_desc</t>
+  </si>
+  <si>
+    <t>total_missing_desc</t>
+  </si>
+  <si>
+    <t>total_injuries_desc</t>
+  </si>
+  <si>
+    <t>total_damage_desc</t>
+  </si>
+  <si>
+    <t>total_houses_destroyed_desc</t>
+  </si>
+  <si>
+    <t>total_houses_damaged_desc</t>
+  </si>
+  <si>
+    <t>ORIG</t>
   </si>
 </sst>
 </file>
@@ -456,9 +533,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -478,8 +552,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,380 +870,479 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD114FB-FD9A-44D8-B328-C296A5B90B93}">
-  <dimension ref="A1:C46"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="26.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="26.140625" style="8"/>
+    <col min="2" max="2" width="34.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="26.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="C2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="D4" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="D15" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="D16" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="D17" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="D18" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="D19" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="D20" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+      <c r="D21" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="D22" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="D24" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="D26" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+      <c r="D28" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="D30" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="D32" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
+      <c r="D34" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
+      <c r="B35" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="D36" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="B37" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="B38" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+      <c r="B39" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
+      <c r="B40" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+      <c r="B41" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
+      <c r="D42" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
+      <c r="B43" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="165.75" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
+      <c r="D44" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="9" t="s">
+      <c r="B45" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="B46" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D46" xr:uid="{FF3B8DFC-6ABD-4C71-9856-5FFC8290B412}">
+    <filterColumn colId="0">
+      <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1196,146 +1370,146 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>20</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>30</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>40</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>50</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>60</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>70</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>80</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>90</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>100</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>110</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4">
+        <v>110</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>120</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>130</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>140</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>150</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>160</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>170</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1354,111 +1528,111 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="74.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="74.42578125" style="2"/>
+    <col min="1" max="1" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="74.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1477,26 +1651,472 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.5703125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="35.5703125" style="6"/>
+    <col min="1" max="1" width="5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="35.5703125" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="144" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79250016-A92D-4B94-97E5-A6BC09D5ED50}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="str">
+        <f>("'"&amp;A2&amp;"',")</f>
+        <v>'ID',</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LOWER(TRIM(A2))</f>
+        <v>id</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" t="str">
+        <f>D2&amp; " = Column("&amp;E2</f>
+        <v>id = Column(Integer</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B19" si="0">("'"&amp;A3&amp;"',")</f>
+        <v>'FLAG_TSUNAMI',</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C19" si="1">LOWER(TRIM(A3))</f>
+        <v>flag_tsunami</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G19" si="2">D3&amp; " = Column("&amp;E3</f>
+        <v>tsunami_fl = Column(String</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>'YEAR',</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>year</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>year = Column(String</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>'EQ_PRIMARY',</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>eq_primary</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>magnitude = Column(Integer</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>'INTENSITY',</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>intensity</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>intensity = Column(Real</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>'COUNTRY',</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>country</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>country = Column(String</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>'STATE',</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>state</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>state = Column(String</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>'LOCATION_NAME',</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>location_name</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>location = Column(String</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>'LATITUDE',</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>latitude</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>lat = Column(Real</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>'LONGITUDE',</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>longitude</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>lng = Column(Real</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>'REGION_CODE',</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>region_code</v>
+      </c>
+      <c r="D12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>region_cd = Column(String</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>'REGION',</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>region</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>region = Column(String</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>'TOTAL_DEATHS_DESCRIPTION',</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>total_deaths_description</v>
+      </c>
+      <c r="D14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>total_deaths_desc = Column(String</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>'TOTAL_MISSING_DESCRIPTION',</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>total_missing_description</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>total_missing_desc = Column(String</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>'TOTAL_INJURIES_DESCRIPTION',</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>total_injuries_description</v>
+      </c>
+      <c r="D16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>total_injuries_desc = Column(String</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>'TOTAL_DAMAGE_DESCRIPTION',</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>total_damage_description</v>
+      </c>
+      <c r="D17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>total_damage_desc = Column(String</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>'TOTAL_HOUSES_DESTROYED_DESCRIPTION',</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>total_houses_destroyed_description</v>
+      </c>
+      <c r="D18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>total_houses_destroyed_desc = Column(String</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>'TOTAL_HOUSES_DAMAGED_DESCRIPTION',</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>total_houses_damaged_description</v>
+      </c>
+      <c r="D19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>total_houses_damaged_desc = Column(String</v>
       </c>
     </row>
   </sheetData>

</xml_diff>